<commit_message>
Adding API oppy and XLS oppy
</commit_message>
<xml_diff>
--- a/main.xlsx
+++ b/main.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="14970" windowHeight="6600" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="14970" windowHeight="6600" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="9" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Price Book" sheetId="12" r:id="rId6"/>
     <sheet name="Price Book Products" sheetId="13" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>description</t>
   </si>
@@ -103,18 +103,6 @@
     <t>Homero Simpson</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>closeDate</t>
-  </si>
-  <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>budget</t>
-  </si>
-  <si>
     <t>Bart Simpson</t>
   </si>
   <si>
@@ -218,6 +206,24 @@
   </si>
   <si>
     <t>FrancoDaniel</t>
+  </si>
+  <si>
+    <t>Close Date</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -327,7 +333,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,7 +638,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,7 +652,7 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
@@ -734,7 +740,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
@@ -746,10 +752,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -815,7 +821,7 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -840,11 +846,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -856,22 +862,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,8 +893,8 @@
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="b">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F2" s="1">
         <v>10000</v>
@@ -896,19 +902,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="9">
         <v>43222</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="b">
-        <v>0</v>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F3" s="1">
         <v>5000</v>
@@ -916,19 +922,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="9">
         <v>43223</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="b">
-        <v>1</v>
+      <c r="E4" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F4" s="1">
         <v>1000</v>
@@ -936,16 +942,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -964,7 +970,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -977,42 +983,42 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="17">
         <v>43446</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F2" s="10">
         <v>2</v>
@@ -1023,19 +1029,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
@@ -1046,19 +1052,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="11">
         <v>43293</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4" s="10">
         <v>2</v>
@@ -1077,11 +1083,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1091,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>21</v>
@@ -1119,13 +1125,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" s="10">
         <v>101</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
@@ -1133,7 +1139,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1143,7 +1149,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1176,7 +1182,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
@@ -1184,15 +1190,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="10" t="b">
         <v>1</v>
@@ -1200,7 +1206,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>1</v>
@@ -1219,7 +1225,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
@@ -1228,18 +1234,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>23</v>
@@ -1250,7 +1256,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>23</v>
@@ -1261,10 +1267,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" s="5">
         <v>40</v>
@@ -1272,10 +1278,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1">
         <v>30</v>

</xml_diff>